<commit_message>
Add Held two layer model runs
</commit_message>
<xml_diff>
--- a/notebooks/rcmip-data-submission-template-ar5ir.xlsx
+++ b/notebooks/rcmip-data-submission-template-ar5ir.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11208"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27F837C5-4129-E748-ACE9-A74DFB38E067}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A8E198-ED6C-2445-AE31-57EF8ECA9567}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" tabRatio="682" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4222,20 +4222,20 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -4632,25 +4632,25 @@
       <c r="B1" s="15"/>
     </row>
     <row r="2" spans="1:13" ht="47.25" customHeight="1">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="79" t="s">
         <v>234</v>
       </c>
-      <c r="B2" s="78"/>
+      <c r="B2" s="79"/>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:13" ht="35.75" customHeight="1">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="78" t="s">
         <v>235</v>
       </c>
-      <c r="B3" s="76"/>
+      <c r="B3" s="78"/>
     </row>
     <row r="4" spans="1:13" ht="61" customHeight="1">
-      <c r="A4" s="77" t="s">
+      <c r="A4" s="80" t="s">
         <v>236</v>
       </c>
-      <c r="B4" s="77"/>
-      <c r="C4" s="79"/>
-      <c r="D4" s="79"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:13" s="4" customFormat="1" ht="6" customHeight="1">
@@ -4669,20 +4669,20 @@
       <c r="M5" s="3"/>
     </row>
     <row r="6" spans="1:13" ht="25.5" customHeight="1">
-      <c r="A6" s="80" t="s">
+      <c r="A6" s="77" t="s">
         <v>76</v>
       </c>
-      <c r="B6" s="80"/>
+      <c r="B6" s="77"/>
     </row>
     <row r="7" spans="1:13" ht="6" customHeight="1">
       <c r="A7" s="17"/>
       <c r="B7" s="17"/>
     </row>
     <row r="8" spans="1:13" s="4" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A8" s="76" t="s">
+      <c r="A8" s="78" t="s">
         <v>848</v>
       </c>
-      <c r="B8" s="76"/>
+      <c r="B8" s="78"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -4696,8 +4696,8 @@
       <c r="M8" s="3"/>
     </row>
     <row r="9" spans="1:13" s="4" customFormat="1" ht="6" customHeight="1">
-      <c r="A9" s="76"/>
-      <c r="B9" s="76"/>
+      <c r="A9" s="78"/>
+      <c r="B9" s="78"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -4711,10 +4711,10 @@
       <c r="M9" s="3"/>
     </row>
     <row r="10" spans="1:13" s="4" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A10" s="76" t="s">
+      <c r="A10" s="78" t="s">
         <v>992</v>
       </c>
-      <c r="B10" s="76"/>
+      <c r="B10" s="78"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -4728,8 +4728,8 @@
       <c r="M10" s="3"/>
     </row>
     <row r="11" spans="1:13" s="4" customFormat="1" ht="6" customHeight="1">
-      <c r="A11" s="76"/>
-      <c r="B11" s="76"/>
+      <c r="A11" s="78"/>
+      <c r="B11" s="78"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -4743,10 +4743,10 @@
       <c r="M11" s="3"/>
     </row>
     <row r="12" spans="1:13" s="4" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A12" s="76" t="s">
+      <c r="A12" s="78" t="s">
         <v>237</v>
       </c>
-      <c r="B12" s="76"/>
+      <c r="B12" s="78"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -4760,8 +4760,8 @@
       <c r="M12" s="3"/>
     </row>
     <row r="13" spans="1:13" s="4" customFormat="1" ht="6" customHeight="1">
-      <c r="A13" s="76"/>
-      <c r="B13" s="76"/>
+      <c r="A13" s="78"/>
+      <c r="B13" s="78"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -4775,10 +4775,10 @@
       <c r="M13" s="3"/>
     </row>
     <row r="14" spans="1:13" s="4" customFormat="1" ht="90" customHeight="1">
-      <c r="A14" s="76" t="s">
+      <c r="A14" s="78" t="s">
         <v>628</v>
       </c>
-      <c r="B14" s="76"/>
+      <c r="B14" s="78"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -4807,10 +4807,10 @@
       <c r="M15" s="3"/>
     </row>
     <row r="16" spans="1:13">
-      <c r="A16" s="80" t="s">
+      <c r="A16" s="77" t="s">
         <v>820</v>
       </c>
-      <c r="B16" s="80"/>
+      <c r="B16" s="77"/>
     </row>
     <row r="17" spans="1:2" ht="26.25" customHeight="1">
       <c r="A17" s="69" t="s">
@@ -4833,10 +4833,10 @@
       <c r="B19" s="17"/>
     </row>
     <row r="20" spans="1:2" ht="27.75" customHeight="1">
-      <c r="A20" s="76" t="s">
+      <c r="A20" s="78" t="s">
         <v>106</v>
       </c>
-      <c r="B20" s="76"/>
+      <c r="B20" s="78"/>
     </row>
     <row r="21" spans="1:2" ht="27.75" customHeight="1">
       <c r="A21" s="72"/>
@@ -4849,10 +4849,10 @@
       <c r="B22" s="72"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="76" t="s">
+      <c r="A23" s="78" t="s">
         <v>1176</v>
       </c>
-      <c r="B23" s="76"/>
+      <c r="B23" s="78"/>
     </row>
     <row r="24" spans="1:2" ht="27.75" customHeight="1">
       <c r="A24" s="68"/>
@@ -4865,10 +4865,10 @@
       <c r="B25" s="68"/>
     </row>
     <row r="26" spans="1:2" ht="88" customHeight="1">
-      <c r="A26" s="76" t="s">
+      <c r="A26" s="78" t="s">
         <v>1032</v>
       </c>
-      <c r="B26" s="76"/>
+      <c r="B26" s="78"/>
     </row>
     <row r="27" spans="1:2" ht="27.75" customHeight="1">
       <c r="A27" s="68"/>
@@ -4947,22 +4947,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A14:B14"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A16:B16"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B17" r:id="rId1" xr:uid="{688D9660-F982-E440-B8DB-8E4CDAF396B8}"/>
@@ -17381,8 +17381,8 @@
   </sheetPr>
   <dimension ref="A1:CM65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.6640625" defaultRowHeight="13"/>
@@ -17663,7 +17663,7 @@
       <c r="A4" s="53"/>
       <c r="B4" s="54" t="str">
         <f>CONCATENATE(C4, D4,"-", E4)</f>
-        <v>ar5ir3box-CMIP6-BCC-CSM2-MR_r1i1p1f1-CALIB</v>
+        <v>ar5ir3box-CMIP6-GISS-E2-2-G_r1i1p1f1-CALIB</v>
       </c>
       <c r="C4" t="s">
         <v>1203</v>
@@ -17672,7 +17672,7 @@
         <v>1208</v>
       </c>
       <c r="E4" t="s">
-        <v>1209</v>
+        <v>1221</v>
       </c>
       <c r="F4">
         <v>3.8883829331771498</v>
@@ -17682,7 +17682,7 @@
       </c>
       <c r="H4" s="28" t="str">
         <f>"Model configuration tuned to "&amp;E4</f>
-        <v>Model configuration tuned to CMIP6-BCC-CSM2-MR_r1i1p1f1-CALIB</v>
+        <v>Model configuration tuned to CMIP6-GISS-E2-2-G_r1i1p1f1-CALIB</v>
       </c>
       <c r="J4" s="28" t="s">
         <v>1205</v>
@@ -17696,16 +17696,16 @@
       <c r="A5" s="53"/>
       <c r="B5" s="54" t="str">
         <f t="shared" ref="B5:B35" si="0">CONCATENATE(C5, ",", D5, ",", E5)</f>
-        <v>ar5ir,2box,CMIP6-NorCPM1_r1i1p1f1-CALIB</v>
+        <v>ar5ir,3box,CMIP6-GISS-E2-1-G_r1i1p1f1-CALIB</v>
       </c>
       <c r="C5" t="s">
         <v>1203</v>
       </c>
       <c r="D5" t="s">
-        <v>1204</v>
+        <v>1208</v>
       </c>
       <c r="E5" t="s">
-        <v>1220</v>
+        <v>1217</v>
       </c>
       <c r="F5">
         <v>4.6604314677678502</v>
@@ -17714,8 +17714,8 @@
         <v>1.65823136256026</v>
       </c>
       <c r="H5" s="28" t="str">
-        <f t="shared" ref="H5:K35" si="1">"Model configuration tuned to "&amp;E5</f>
-        <v>Model configuration tuned to CMIP6-NorCPM1_r1i1p1f1-CALIB</v>
+        <f t="shared" ref="H5:H35" si="1">"Model configuration tuned to "&amp;E5</f>
+        <v>Model configuration tuned to CMIP6-GISS-E2-1-G_r1i1p1f1-CALIB</v>
       </c>
       <c r="J5" s="28" t="str">
         <f>J4</f>
@@ -17731,7 +17731,7 @@
       <c r="A6" s="53"/>
       <c r="B6" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,2box,CMIP6-GISS-E2-1-G_r1i1p1f1-CALIB</v>
+        <v>ar5ir,2box,CMIP6-NorESM2-LM_r1i1p1f1-CALIB</v>
       </c>
       <c r="C6" t="s">
         <v>1203</v>
@@ -17740,7 +17740,7 @@
         <v>1204</v>
       </c>
       <c r="E6" t="s">
-        <v>1217</v>
+        <v>1222</v>
       </c>
       <c r="F6">
         <v>4.7749213573198501</v>
@@ -17750,7 +17750,7 @@
       </c>
       <c r="H6" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-GISS-E2-1-G_r1i1p1f1-CALIB</v>
+        <v>Model configuration tuned to CMIP6-NorESM2-LM_r1i1p1f1-CALIB</v>
       </c>
       <c r="J6" s="28" t="str">
         <f t="shared" ref="J6:J35" si="2">J5</f>
@@ -17766,7 +17766,7 @@
       <c r="A7" s="53"/>
       <c r="B7" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,3box,CMIP6-GISS-E2-1-G_r1i1p1f1-CALIB</v>
+        <v>ar5ir,3box,CMIP6-NorESM2-LM_r1i1p1f1-CALIB</v>
       </c>
       <c r="C7" t="s">
         <v>1203</v>
@@ -17775,7 +17775,7 @@
         <v>1208</v>
       </c>
       <c r="E7" t="s">
-        <v>1217</v>
+        <v>1222</v>
       </c>
       <c r="F7">
         <v>4.8676924657394203</v>
@@ -17785,7 +17785,7 @@
       </c>
       <c r="H7" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-GISS-E2-1-G_r1i1p1f1-CALIB</v>
+        <v>Model configuration tuned to CMIP6-NorESM2-LM_r1i1p1f1-CALIB</v>
       </c>
       <c r="J7" s="28" t="str">
         <f t="shared" si="2"/>
@@ -17801,7 +17801,7 @@
       <c r="A8" s="53"/>
       <c r="B8" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,3box,CMIP6-GISS-E2-1-H_r1i1p1f1-CALIB</v>
+        <v>ar5ir,3box,CMIP6-NorCPM1_r1i1p1f1-CALIB</v>
       </c>
       <c r="C8" t="s">
         <v>1203</v>
@@ -17810,7 +17810,7 @@
         <v>1208</v>
       </c>
       <c r="E8" t="s">
-        <v>1211</v>
+        <v>1220</v>
       </c>
       <c r="F8">
         <v>5.6400004762161302</v>
@@ -17820,7 +17820,7 @@
       </c>
       <c r="H8" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-GISS-E2-1-H_r1i1p1f1-CALIB</v>
+        <v>Model configuration tuned to CMIP6-NorCPM1_r1i1p1f1-CALIB</v>
       </c>
       <c r="J8" s="28" t="str">
         <f t="shared" si="2"/>
@@ -17871,16 +17871,16 @@
       <c r="A10" s="53"/>
       <c r="B10" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,3box,CMIP6-IPSL-CM6A-LR_r1i1p1f1-CALIB</v>
+        <v>ar5ir,2box,CMIP6-NorCPM1_r1i1p1f1-CALIB</v>
       </c>
       <c r="C10" t="s">
         <v>1203</v>
       </c>
       <c r="D10" t="s">
-        <v>1208</v>
+        <v>1204</v>
       </c>
       <c r="E10" t="s">
-        <v>1216</v>
+        <v>1220</v>
       </c>
       <c r="F10">
         <v>5.9849619111386696</v>
@@ -17890,7 +17890,7 @@
       </c>
       <c r="H10" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-IPSL-CM6A-LR_r1i1p1f1-CALIB</v>
+        <v>Model configuration tuned to CMIP6-NorCPM1_r1i1p1f1-CALIB</v>
       </c>
       <c r="J10" s="28" t="str">
         <f t="shared" si="2"/>
@@ -17906,7 +17906,7 @@
       <c r="A11" s="53"/>
       <c r="B11" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,2box,CMIP6-BCC-ESM1_r1i1p1f1-CALIB</v>
+        <v>ar5ir,2box,CMIP6-GISS-E2-1-G_r1i1p1f1-CALIB</v>
       </c>
       <c r="C11" t="s">
         <v>1203</v>
@@ -17915,7 +17915,7 @@
         <v>1204</v>
       </c>
       <c r="E11" t="s">
-        <v>1210</v>
+        <v>1217</v>
       </c>
       <c r="F11">
         <v>6.15826724672542</v>
@@ -17925,7 +17925,7 @@
       </c>
       <c r="H11" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-BCC-ESM1_r1i1p1f1-CALIB</v>
+        <v>Model configuration tuned to CMIP6-GISS-E2-1-G_r1i1p1f1-CALIB</v>
       </c>
       <c r="J11" s="28" t="str">
         <f t="shared" si="2"/>
@@ -17941,7 +17941,7 @@
       <c r="A12" s="53"/>
       <c r="B12" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,2box,CMIP6-UKESM1-0-LL_r1i1p1f2-CALIB</v>
+        <v>ar5ir,2box,CMIP6-BCC-ESM1_r1i1p1f1-CALIB</v>
       </c>
       <c r="C12" t="s">
         <v>1203</v>
@@ -17950,7 +17950,7 @@
         <v>1204</v>
       </c>
       <c r="E12" t="s">
-        <v>1218</v>
+        <v>1210</v>
       </c>
       <c r="F12">
         <v>6.1648418835021896</v>
@@ -17960,7 +17960,7 @@
       </c>
       <c r="H12" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-UKESM1-0-LL_r1i1p1f2-CALIB</v>
+        <v>Model configuration tuned to CMIP6-BCC-ESM1_r1i1p1f1-CALIB</v>
       </c>
       <c r="J12" s="28" t="str">
         <f t="shared" si="2"/>
@@ -17976,7 +17976,7 @@
       <c r="A13" s="53"/>
       <c r="B13" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,3box,CMIP6-CNRM-ESM2-1_r1i1p1f2-CALIB</v>
+        <v>ar5ir,3box,CMIP6-BCC-ESM1_r1i1p1f1-CALIB</v>
       </c>
       <c r="C13" t="s">
         <v>1203</v>
@@ -17985,7 +17985,7 @@
         <v>1208</v>
       </c>
       <c r="E13" t="s">
-        <v>1215</v>
+        <v>1210</v>
       </c>
       <c r="F13">
         <v>6.6063084373020704</v>
@@ -17995,7 +17995,7 @@
       </c>
       <c r="H13" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-CNRM-ESM2-1_r1i1p1f2-CALIB</v>
+        <v>Model configuration tuned to CMIP6-BCC-ESM1_r1i1p1f1-CALIB</v>
       </c>
       <c r="J13" s="28" t="str">
         <f t="shared" si="2"/>
@@ -18011,7 +18011,7 @@
       <c r="A14" s="38"/>
       <c r="B14" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,3box,CMIP6-NorESM2-LM_r1i1p1f1-CALIB</v>
+        <v>ar5ir,3box,CMIP6-MPI-ESM1-2-HR_r1i1p1f1-CALIB</v>
       </c>
       <c r="C14" t="s">
         <v>1203</v>
@@ -18020,7 +18020,7 @@
         <v>1208</v>
       </c>
       <c r="E14" t="s">
-        <v>1222</v>
+        <v>1212</v>
       </c>
       <c r="F14">
         <v>6.7808043875969304</v>
@@ -18030,7 +18030,7 @@
       </c>
       <c r="H14" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-NorESM2-LM_r1i1p1f1-CALIB</v>
+        <v>Model configuration tuned to CMIP6-MPI-ESM1-2-HR_r1i1p1f1-CALIB</v>
       </c>
       <c r="J14" s="28" t="str">
         <f t="shared" si="2"/>
@@ -18045,7 +18045,7 @@
     <row r="15" spans="1:91" ht="36.75" customHeight="1" thickBot="1">
       <c r="B15" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,2box,CMIP6-CESM2_r1i1p1f1-CALIB</v>
+        <v>ar5ir,2box,CMIP6-MPI-ESM1-2-HR_r1i1p1f1-CALIB</v>
       </c>
       <c r="C15" t="s">
         <v>1203</v>
@@ -18054,7 +18054,7 @@
         <v>1204</v>
       </c>
       <c r="E15" t="s">
-        <v>1223</v>
+        <v>1212</v>
       </c>
       <c r="F15">
         <v>6.7975907508722999</v>
@@ -18064,7 +18064,7 @@
       </c>
       <c r="H15" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-CESM2_r1i1p1f1-CALIB</v>
+        <v>Model configuration tuned to CMIP6-MPI-ESM1-2-HR_r1i1p1f1-CALIB</v>
       </c>
       <c r="J15" s="28" t="str">
         <f t="shared" si="2"/>
@@ -18078,7 +18078,7 @@
     <row r="16" spans="1:91" ht="36.75" customHeight="1" thickBot="1">
       <c r="B16" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,2box,CMIP6-CESM2-WACCM_r1i1p1f1-CALIB</v>
+        <v>ar5ir,2box,CMIP6-GISS-E2-1-H_r1i1p1f1-CALIB</v>
       </c>
       <c r="C16" t="s">
         <v>1203</v>
@@ -18087,7 +18087,7 @@
         <v>1204</v>
       </c>
       <c r="E16" t="s">
-        <v>1224</v>
+        <v>1211</v>
       </c>
       <c r="F16">
         <v>6.86884689256072</v>
@@ -18097,7 +18097,7 @@
       </c>
       <c r="H16" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-CESM2-WACCM_r1i1p1f1-CALIB</v>
+        <v>Model configuration tuned to CMIP6-GISS-E2-1-H_r1i1p1f1-CALIB</v>
       </c>
       <c r="J16" s="28" t="str">
         <f t="shared" si="2"/>
@@ -18111,7 +18111,7 @@
     <row r="17" spans="2:11" ht="36.75" customHeight="1" thickBot="1">
       <c r="B17" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,3box,CMIP6-NorCPM1_r1i1p1f1-CALIB</v>
+        <v>ar5ir,3box,CMIP6-GISS-E2-1-H_r1i1p1f1-CALIB</v>
       </c>
       <c r="C17" t="s">
         <v>1203</v>
@@ -18120,7 +18120,7 @@
         <v>1208</v>
       </c>
       <c r="E17" t="s">
-        <v>1220</v>
+        <v>1211</v>
       </c>
       <c r="F17">
         <v>7.0265561916764101</v>
@@ -18130,7 +18130,7 @@
       </c>
       <c r="H17" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-NorCPM1_r1i1p1f1-CALIB</v>
+        <v>Model configuration tuned to CMIP6-GISS-E2-1-H_r1i1p1f1-CALIB</v>
       </c>
       <c r="J17" s="28" t="str">
         <f t="shared" si="2"/>
@@ -18144,7 +18144,7 @@
     <row r="18" spans="2:11" ht="36.75" customHeight="1" thickBot="1">
       <c r="B18" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,3box,CMIP6-MPI-ESM1-2-HR_r1i1p1f1-CALIB</v>
+        <v>ar5ir,3box,CMIP6-BCC-CSM2-MR_r1i1p1f1-CALIB</v>
       </c>
       <c r="C18" t="s">
         <v>1203</v>
@@ -18153,7 +18153,7 @@
         <v>1208</v>
       </c>
       <c r="E18" t="s">
-        <v>1212</v>
+        <v>1209</v>
       </c>
       <c r="F18">
         <v>7.1707996134210399</v>
@@ -18163,7 +18163,7 @@
       </c>
       <c r="H18" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-MPI-ESM1-2-HR_r1i1p1f1-CALIB</v>
+        <v>Model configuration tuned to CMIP6-BCC-CSM2-MR_r1i1p1f1-CALIB</v>
       </c>
       <c r="J18" s="28" t="str">
         <f t="shared" si="2"/>
@@ -18177,7 +18177,7 @@
     <row r="19" spans="2:11" ht="36.75" customHeight="1" thickBot="1">
       <c r="B19" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,2box,CMIP6-MPI-ESM1-2-HR_r1i1p1f1-CALIB</v>
+        <v>ar5ir,2box,CMIP6-BCC-CSM2-MR_r1i1p1f1-CALIB</v>
       </c>
       <c r="C19" t="s">
         <v>1203</v>
@@ -18186,7 +18186,7 @@
         <v>1204</v>
       </c>
       <c r="E19" t="s">
-        <v>1212</v>
+        <v>1209</v>
       </c>
       <c r="F19">
         <v>7.4359428125203797</v>
@@ -18196,7 +18196,7 @@
       </c>
       <c r="H19" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-MPI-ESM1-2-HR_r1i1p1f1-CALIB</v>
+        <v>Model configuration tuned to CMIP6-BCC-CSM2-MR_r1i1p1f1-CALIB</v>
       </c>
       <c r="J19" s="28" t="str">
         <f t="shared" si="2"/>
@@ -18210,16 +18210,16 @@
     <row r="20" spans="2:11" ht="36.75" customHeight="1" thickBot="1">
       <c r="B20" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,3box,CMIP6-UKESM1-0-LL_r1i1p1f2-CALIB</v>
+        <v>ar5ir,2box,CMIP6-CESM2-WACCM_r1i1p1f1-CALIB</v>
       </c>
       <c r="C20" t="s">
         <v>1203</v>
       </c>
       <c r="D20" t="s">
-        <v>1208</v>
+        <v>1204</v>
       </c>
       <c r="E20" t="s">
-        <v>1218</v>
+        <v>1224</v>
       </c>
       <c r="F20">
         <v>7.4897386925168199</v>
@@ -18229,7 +18229,7 @@
       </c>
       <c r="H20" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-UKESM1-0-LL_r1i1p1f2-CALIB</v>
+        <v>Model configuration tuned to CMIP6-CESM2-WACCM_r1i1p1f1-CALIB</v>
       </c>
       <c r="J20" s="28" t="str">
         <f t="shared" si="2"/>
@@ -18243,16 +18243,16 @@
     <row r="21" spans="2:11" ht="36.75" customHeight="1" thickBot="1">
       <c r="B21" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,3box,CMIP6-CESM2_r1i1p1f1-CALIB</v>
+        <v>ar5ir,2box,CMIP6-CNRM-ESM2-1_r1i1p1f2-CALIB</v>
       </c>
       <c r="C21" t="s">
         <v>1203</v>
       </c>
       <c r="D21" t="s">
-        <v>1208</v>
+        <v>1204</v>
       </c>
       <c r="E21" t="s">
-        <v>1223</v>
+        <v>1215</v>
       </c>
       <c r="F21">
         <v>7.8002326489343403</v>
@@ -18262,7 +18262,7 @@
       </c>
       <c r="H21" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-CESM2_r1i1p1f1-CALIB</v>
+        <v>Model configuration tuned to CMIP6-CNRM-ESM2-1_r1i1p1f2-CALIB</v>
       </c>
       <c r="J21" s="28" t="str">
         <f t="shared" si="2"/>
@@ -18276,16 +18276,16 @@
     <row r="22" spans="2:11" ht="36.75" customHeight="1" thickBot="1">
       <c r="B22" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,2box,CMIP6-EC-Earth3-Veg_r1i1p1f1-CALIB</v>
+        <v>ar5ir,3box,CMIP6-CNRM-ESM2-1_r1i1p1f2-CALIB</v>
       </c>
       <c r="C22" t="s">
         <v>1203</v>
       </c>
       <c r="D22" t="s">
-        <v>1204</v>
+        <v>1208</v>
       </c>
       <c r="E22" t="s">
-        <v>1219</v>
+        <v>1215</v>
       </c>
       <c r="F22">
         <v>7.9858149852556002</v>
@@ -18295,7 +18295,7 @@
       </c>
       <c r="H22" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-EC-Earth3-Veg_r1i1p1f1-CALIB</v>
+        <v>Model configuration tuned to CMIP6-CNRM-ESM2-1_r1i1p1f2-CALIB</v>
       </c>
       <c r="J22" s="28" t="str">
         <f t="shared" si="2"/>
@@ -18309,7 +18309,7 @@
     <row r="23" spans="2:11" ht="36.75" customHeight="1" thickBot="1">
       <c r="B23" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,3box,CMIP6-BCC-ESM1_r1i1p1f1-CALIB</v>
+        <v>ar5ir,3box,CMIP6-CESM2-WACCM_r1i1p1f1-CALIB</v>
       </c>
       <c r="C23" t="s">
         <v>1203</v>
@@ -18318,7 +18318,7 @@
         <v>1208</v>
       </c>
       <c r="E23" t="s">
-        <v>1210</v>
+        <v>1224</v>
       </c>
       <c r="F23">
         <v>8.23432269905312</v>
@@ -18328,7 +18328,7 @@
       </c>
       <c r="H23" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-BCC-ESM1_r1i1p1f1-CALIB</v>
+        <v>Model configuration tuned to CMIP6-CESM2-WACCM_r1i1p1f1-CALIB</v>
       </c>
       <c r="J23" s="28" t="str">
         <f t="shared" si="2"/>
@@ -18342,16 +18342,16 @@
     <row r="24" spans="2:11" ht="36.75" customHeight="1" thickBot="1">
       <c r="B24" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,2box,CMIP6-CNRM-ESM2-1_r1i1p1f2-CALIB</v>
+        <v>ar5ir,3box,CMIP6-CESM2_r1i1p1f1-CALIB</v>
       </c>
       <c r="C24" t="s">
         <v>1203</v>
       </c>
       <c r="D24" t="s">
-        <v>1204</v>
+        <v>1208</v>
       </c>
       <c r="E24" t="s">
-        <v>1215</v>
+        <v>1223</v>
       </c>
       <c r="F24">
         <v>8.3803876364999894</v>
@@ -18361,7 +18361,7 @@
       </c>
       <c r="H24" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-CNRM-ESM2-1_r1i1p1f2-CALIB</v>
+        <v>Model configuration tuned to CMIP6-CESM2_r1i1p1f1-CALIB</v>
       </c>
       <c r="J24" s="28" t="str">
         <f t="shared" si="2"/>
@@ -18375,7 +18375,7 @@
     <row r="25" spans="2:11" ht="36.75" customHeight="1" thickBot="1">
       <c r="B25" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,2box,CMIP6-NorESM2-LM_r1i1p1f1-CALIB</v>
+        <v>ar5ir,2box,CMIP6-CESM2_r1i1p1f1-CALIB</v>
       </c>
       <c r="C25" t="s">
         <v>1203</v>
@@ -18384,7 +18384,7 @@
         <v>1204</v>
       </c>
       <c r="E25" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="F25">
         <v>8.5042228866140697</v>
@@ -18394,7 +18394,7 @@
       </c>
       <c r="H25" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-NorESM2-LM_r1i1p1f1-CALIB</v>
+        <v>Model configuration tuned to CMIP6-CESM2_r1i1p1f1-CALIB</v>
       </c>
       <c r="J25" s="28" t="str">
         <f t="shared" si="2"/>
@@ -18408,7 +18408,7 @@
     <row r="26" spans="2:11" ht="36.75" customHeight="1" thickBot="1">
       <c r="B26" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,3box,CMIP6-GISS-E2-2-G_r1i1p1f1-CALIB</v>
+        <v>ar5ir,3box,CMIP6-CNRM-CM6-1_r1i1p1f2-CALIB</v>
       </c>
       <c r="C26" t="s">
         <v>1203</v>
@@ -18417,7 +18417,7 @@
         <v>1208</v>
       </c>
       <c r="E26" t="s">
-        <v>1221</v>
+        <v>1213</v>
       </c>
       <c r="F26">
         <v>8.8187245100804397</v>
@@ -18427,7 +18427,7 @@
       </c>
       <c r="H26" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-GISS-E2-2-G_r1i1p1f1-CALIB</v>
+        <v>Model configuration tuned to CMIP6-CNRM-CM6-1_r1i1p1f2-CALIB</v>
       </c>
       <c r="J26" s="28" t="str">
         <f t="shared" si="2"/>
@@ -18474,7 +18474,7 @@
     <row r="28" spans="2:11" ht="36.75" customHeight="1" thickBot="1">
       <c r="B28" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,2box,CMIP6-GISS-E2-1-H_r1i1p1f1-CALIB</v>
+        <v>ar5ir,2box,CMIP6-IPSL-CM6A-LR_r1i1p1f1-CALIB</v>
       </c>
       <c r="C28" t="s">
         <v>1203</v>
@@ -18483,7 +18483,7 @@
         <v>1204</v>
       </c>
       <c r="E28" t="s">
-        <v>1211</v>
+        <v>1216</v>
       </c>
       <c r="F28">
         <v>10.051406813280201</v>
@@ -18493,7 +18493,7 @@
       </c>
       <c r="H28" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-GISS-E2-1-H_r1i1p1f1-CALIB</v>
+        <v>Model configuration tuned to CMIP6-IPSL-CM6A-LR_r1i1p1f1-CALIB</v>
       </c>
       <c r="J28" s="28" t="str">
         <f t="shared" si="2"/>
@@ -18507,16 +18507,16 @@
     <row r="29" spans="2:11" ht="36.75" customHeight="1" thickBot="1">
       <c r="B29" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,2box,CMIP6-CanESM5_r1i1p1f1-CALIB</v>
+        <v>ar5ir,3box,CMIP6-EC-Earth3-Veg_r1i1p1f1-CALIB</v>
       </c>
       <c r="C29" t="s">
         <v>1203</v>
       </c>
       <c r="D29" t="s">
-        <v>1204</v>
+        <v>1208</v>
       </c>
       <c r="E29" t="s">
-        <v>1214</v>
+        <v>1219</v>
       </c>
       <c r="F29">
         <v>10.324524704285899</v>
@@ -18526,7 +18526,7 @@
       </c>
       <c r="H29" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-CanESM5_r1i1p1f1-CALIB</v>
+        <v>Model configuration tuned to CMIP6-EC-Earth3-Veg_r1i1p1f1-CALIB</v>
       </c>
       <c r="J29" s="28" t="str">
         <f t="shared" si="2"/>
@@ -18540,7 +18540,7 @@
     <row r="30" spans="2:11" ht="36.75" customHeight="1" thickBot="1">
       <c r="B30" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,2box,CMIP6-BCC-CSM2-MR_r1i1p1f1-CALIB</v>
+        <v>ar5ir,2box,CMIP6-EC-Earth3-Veg_r1i1p1f1-CALIB</v>
       </c>
       <c r="C30" t="s">
         <v>1203</v>
@@ -18549,7 +18549,7 @@
         <v>1204</v>
       </c>
       <c r="E30" t="s">
-        <v>1209</v>
+        <v>1219</v>
       </c>
       <c r="F30">
         <v>10.541577456198601</v>
@@ -18559,7 +18559,7 @@
       </c>
       <c r="H30" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-BCC-CSM2-MR_r1i1p1f1-CALIB</v>
+        <v>Model configuration tuned to CMIP6-EC-Earth3-Veg_r1i1p1f1-CALIB</v>
       </c>
       <c r="J30" s="28" t="str">
         <f t="shared" si="2"/>
@@ -18573,7 +18573,7 @@
     <row r="31" spans="2:11" ht="36.75" customHeight="1" thickBot="1">
       <c r="B31" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,3box,CMIP6-EC-Earth3-Veg_r1i1p1f1-CALIB</v>
+        <v>ar5ir,3box,CMIP6-IPSL-CM6A-LR_r1i1p1f1-CALIB</v>
       </c>
       <c r="C31" t="s">
         <v>1203</v>
@@ -18582,7 +18582,7 @@
         <v>1208</v>
       </c>
       <c r="E31" t="s">
-        <v>1219</v>
+        <v>1216</v>
       </c>
       <c r="F31">
         <v>11.081261663595701</v>
@@ -18592,7 +18592,7 @@
       </c>
       <c r="H31" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-EC-Earth3-Veg_r1i1p1f1-CALIB</v>
+        <v>Model configuration tuned to CMIP6-IPSL-CM6A-LR_r1i1p1f1-CALIB</v>
       </c>
       <c r="J31" s="28" t="str">
         <f t="shared" si="2"/>
@@ -18606,7 +18606,7 @@
     <row r="32" spans="2:11" ht="36.75" customHeight="1" thickBot="1">
       <c r="B32" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,3box,CMIP6-CanESM5_r1i1p1f1-CALIB</v>
+        <v>ar5ir,3box,CMIP6-UKESM1-0-LL_r1i1p1f2-CALIB</v>
       </c>
       <c r="C32" t="s">
         <v>1203</v>
@@ -18615,7 +18615,7 @@
         <v>1208</v>
       </c>
       <c r="E32" t="s">
-        <v>1214</v>
+        <v>1218</v>
       </c>
       <c r="F32">
         <v>11.121920885669599</v>
@@ -18625,7 +18625,7 @@
       </c>
       <c r="H32" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-CanESM5_r1i1p1f1-CALIB</v>
+        <v>Model configuration tuned to CMIP6-UKESM1-0-LL_r1i1p1f2-CALIB</v>
       </c>
       <c r="J32" s="28" t="str">
         <f t="shared" si="2"/>
@@ -18639,16 +18639,16 @@
     <row r="33" spans="2:11" ht="36.75" customHeight="1" thickBot="1">
       <c r="B33" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,3box,CMIP6-CNRM-CM6-1_r1i1p1f2-CALIB</v>
+        <v>ar5ir,2box,CMIP6-CanESM5_r1i1p1f1-CALIB</v>
       </c>
       <c r="C33" t="s">
         <v>1203</v>
       </c>
       <c r="D33" t="s">
-        <v>1208</v>
+        <v>1204</v>
       </c>
       <c r="E33" t="s">
-        <v>1213</v>
+        <v>1214</v>
       </c>
       <c r="F33">
         <v>11.3932405906894</v>
@@ -18658,7 +18658,7 @@
       </c>
       <c r="H33" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-CNRM-CM6-1_r1i1p1f2-CALIB</v>
+        <v>Model configuration tuned to CMIP6-CanESM5_r1i1p1f1-CALIB</v>
       </c>
       <c r="J33" s="28" t="str">
         <f t="shared" si="2"/>
@@ -18672,7 +18672,7 @@
     <row r="34" spans="2:11" ht="36.75" customHeight="1" thickBot="1">
       <c r="B34" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,3box,CMIP6-CESM2-WACCM_r1i1p1f1-CALIB</v>
+        <v>ar5ir,3box,CMIP6-CanESM5_r1i1p1f1-CALIB</v>
       </c>
       <c r="C34" t="s">
         <v>1203</v>
@@ -18681,7 +18681,7 @@
         <v>1208</v>
       </c>
       <c r="E34" t="s">
-        <v>1224</v>
+        <v>1214</v>
       </c>
       <c r="F34">
         <v>11.487074387838099</v>
@@ -18691,7 +18691,7 @@
       </c>
       <c r="H34" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-CESM2-WACCM_r1i1p1f1-CALIB</v>
+        <v>Model configuration tuned to CMIP6-CanESM5_r1i1p1f1-CALIB</v>
       </c>
       <c r="J34" s="28" t="str">
         <f t="shared" si="2"/>
@@ -18705,7 +18705,7 @@
     <row r="35" spans="2:11" ht="36.75" customHeight="1">
       <c r="B35" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,2box,CMIP6-IPSL-CM6A-LR_r1i1p1f1-CALIB</v>
+        <v>ar5ir,2box,CMIP6-UKESM1-0-LL_r1i1p1f2-CALIB</v>
       </c>
       <c r="C35" t="s">
         <v>1203</v>
@@ -18714,7 +18714,7 @@
         <v>1204</v>
       </c>
       <c r="E35" t="s">
-        <v>1216</v>
+        <v>1218</v>
       </c>
       <c r="F35">
         <v>12.142995499498401</v>
@@ -18724,7 +18724,7 @@
       </c>
       <c r="H35" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-IPSL-CM6A-LR_r1i1p1f1-CALIB</v>
+        <v>Model configuration tuned to CMIP6-UKESM1-0-LL_r1i1p1f2-CALIB</v>
       </c>
       <c r="J35" s="28" t="str">
         <f t="shared" si="2"/>

</xml_diff>

<commit_message>
Add default setups too
</commit_message>
<xml_diff>
--- a/notebooks/rcmip-data-submission-template-ar5ir.xlsx
+++ b/notebooks/rcmip-data-submission-template-ar5ir.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11208"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A8E198-ED6C-2445-AE31-57EF8ECA9567}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA983CA-A05D-0A4F-A822-C8EE36661313}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" tabRatio="682" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2080" uniqueCount="1225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2086" uniqueCount="1226">
   <si>
     <t>Category</t>
   </si>
@@ -3789,6 +3789,9 @@
   </si>
   <si>
     <t>CMIP6-CESM2-WACCM_r1i1p1f1-CALIB</t>
+  </si>
+  <si>
+    <t>ECS-3K</t>
   </si>
 </sst>
 </file>
@@ -17381,9 +17384,7 @@
   </sheetPr>
   <dimension ref="A1:CM65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.6640625" defaultRowHeight="13"/>
   <cols>
@@ -17663,26 +17664,26 @@
       <c r="A4" s="53"/>
       <c r="B4" s="54" t="str">
         <f>CONCATENATE(C4, D4,"-", E4)</f>
-        <v>ar5ir3box-CMIP6-GISS-E2-2-G_r1i1p1f1-CALIB</v>
+        <v>ar5ir2box-ECS-3K</v>
       </c>
       <c r="C4" t="s">
         <v>1203</v>
       </c>
       <c r="D4" t="s">
-        <v>1208</v>
+        <v>1204</v>
       </c>
       <c r="E4" t="s">
-        <v>1221</v>
+        <v>1225</v>
       </c>
       <c r="F4">
-        <v>3.8883829331771498</v>
+        <v>2.992</v>
       </c>
       <c r="G4">
-        <v>1.9208970104027601</v>
+        <v>2.06925197419908</v>
       </c>
       <c r="H4" s="28" t="str">
         <f>"Model configuration tuned to "&amp;E4</f>
-        <v>Model configuration tuned to CMIP6-GISS-E2-2-G_r1i1p1f1-CALIB</v>
+        <v>Model configuration tuned to ECS-3K</v>
       </c>
       <c r="J4" s="28" t="s">
         <v>1205</v>
@@ -17695,8 +17696,8 @@
     <row r="5" spans="1:91" ht="36.75" customHeight="1" thickBot="1">
       <c r="A5" s="53"/>
       <c r="B5" s="54" t="str">
-        <f t="shared" ref="B5:B35" si="0">CONCATENATE(C5, ",", D5, ",", E5)</f>
-        <v>ar5ir,3box,CMIP6-GISS-E2-1-G_r1i1p1f1-CALIB</v>
+        <f t="shared" ref="B5:B37" si="0">CONCATENATE(C5, ",", D5, ",", E5)</f>
+        <v>ar5ir,3box,ECS-3K</v>
       </c>
       <c r="C5" t="s">
         <v>1203</v>
@@ -17705,17 +17706,17 @@
         <v>1208</v>
       </c>
       <c r="E5" t="s">
-        <v>1217</v>
+        <v>1225</v>
       </c>
       <c r="F5">
-        <v>4.6604314677678502</v>
+        <v>2.992</v>
       </c>
       <c r="G5">
-        <v>1.65823136256026</v>
+        <v>2.1929936881334799</v>
       </c>
       <c r="H5" s="28" t="str">
-        <f t="shared" ref="H5:H35" si="1">"Model configuration tuned to "&amp;E5</f>
-        <v>Model configuration tuned to CMIP6-GISS-E2-1-G_r1i1p1f1-CALIB</v>
+        <f t="shared" ref="H5:H37" si="1">"Model configuration tuned to "&amp;E5</f>
+        <v>Model configuration tuned to ECS-3K</v>
       </c>
       <c r="J5" s="28" t="str">
         <f>J4</f>
@@ -17731,7 +17732,7 @@
       <c r="A6" s="53"/>
       <c r="B6" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,2box,CMIP6-NorESM2-LM_r1i1p1f1-CALIB</v>
+        <v>ar5ir,2box,CMIP6-BCC-CSM2-MR_r1i1p1f1-CALIB</v>
       </c>
       <c r="C6" t="s">
         <v>1203</v>
@@ -17740,24 +17741,24 @@
         <v>1204</v>
       </c>
       <c r="E6" t="s">
-        <v>1222</v>
+        <v>1209</v>
       </c>
       <c r="F6">
-        <v>4.7749213573198501</v>
+        <v>7.3484233453979204</v>
       </c>
       <c r="G6">
-        <v>1.6458078758072401</v>
+        <v>1.92515243525194</v>
       </c>
       <c r="H6" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-NorESM2-LM_r1i1p1f1-CALIB</v>
+        <v>Model configuration tuned to CMIP6-BCC-CSM2-MR_r1i1p1f1-CALIB</v>
       </c>
       <c r="J6" s="28" t="str">
-        <f t="shared" ref="J6:J35" si="2">J5</f>
+        <f t="shared" ref="J6:J37" si="2">J5</f>
         <v>Zebedee Nicholls (zebedee.nicholls@climate-energy-college.org)</v>
       </c>
       <c r="K6" s="30" t="str">
-        <f t="shared" ref="K6:K35" si="3">K5</f>
+        <f t="shared" ref="K6:K37" si="3">K5</f>
         <v>AR5 WG1 Ch.8 SM</v>
       </c>
       <c r="L6" s="32"/>
@@ -17766,26 +17767,26 @@
       <c r="A7" s="53"/>
       <c r="B7" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,3box,CMIP6-NorESM2-LM_r1i1p1f1-CALIB</v>
+        <v>ar5ir,2box,CMIP6-BCC-ESM1_r1i1p1f1-CALIB</v>
       </c>
       <c r="C7" t="s">
         <v>1203</v>
       </c>
       <c r="D7" t="s">
-        <v>1208</v>
+        <v>1204</v>
       </c>
       <c r="E7" t="s">
-        <v>1222</v>
+        <v>1210</v>
       </c>
       <c r="F7">
-        <v>4.8676924657394203</v>
+        <v>15.298255293919899</v>
       </c>
       <c r="G7">
-        <v>1.7327607978922901</v>
+        <v>1.8325969909875901</v>
       </c>
       <c r="H7" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-NorESM2-LM_r1i1p1f1-CALIB</v>
+        <v>Model configuration tuned to CMIP6-BCC-ESM1_r1i1p1f1-CALIB</v>
       </c>
       <c r="J7" s="28" t="str">
         <f t="shared" si="2"/>
@@ -17801,26 +17802,26 @@
       <c r="A8" s="53"/>
       <c r="B8" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,3box,CMIP6-NorCPM1_r1i1p1f1-CALIB</v>
+        <v>ar5ir,2box,CMIP6-CESM2-WACCM_r1i1p1f1-CALIB</v>
       </c>
       <c r="C8" t="s">
         <v>1203</v>
       </c>
       <c r="D8" t="s">
-        <v>1208</v>
+        <v>1204</v>
       </c>
       <c r="E8" t="s">
-        <v>1220</v>
+        <v>1224</v>
       </c>
       <c r="F8">
-        <v>5.6400004762161302</v>
+        <v>4.6383329518360004</v>
       </c>
       <c r="G8">
-        <v>1.90788994550314</v>
+        <v>2.2237921821689302</v>
       </c>
       <c r="H8" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-NorCPM1_r1i1p1f1-CALIB</v>
+        <v>Model configuration tuned to CMIP6-CESM2-WACCM_r1i1p1f1-CALIB</v>
       </c>
       <c r="J8" s="28" t="str">
         <f t="shared" si="2"/>
@@ -17836,7 +17837,7 @@
       <c r="A9" s="53"/>
       <c r="B9" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,2box,CMIP6-GISS-E2-2-G_r1i1p1f1-CALIB</v>
+        <v>ar5ir,2box,CMIP6-CESM2_r1i1p1f1-CALIB</v>
       </c>
       <c r="C9" t="s">
         <v>1203</v>
@@ -17845,17 +17846,17 @@
         <v>1204</v>
       </c>
       <c r="E9" t="s">
-        <v>1221</v>
+        <v>1223</v>
       </c>
       <c r="F9">
-        <v>5.7544858730519701</v>
+        <v>5.3979711341104002</v>
       </c>
       <c r="G9">
-        <v>1.5786320593465899</v>
+        <v>2.37905354300025</v>
       </c>
       <c r="H9" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-GISS-E2-2-G_r1i1p1f1-CALIB</v>
+        <v>Model configuration tuned to CMIP6-CESM2_r1i1p1f1-CALIB</v>
       </c>
       <c r="J9" s="28" t="str">
         <f t="shared" si="2"/>
@@ -17871,7 +17872,7 @@
       <c r="A10" s="53"/>
       <c r="B10" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,2box,CMIP6-NorCPM1_r1i1p1f1-CALIB</v>
+        <v>ar5ir,2box,CMIP6-CNRM-CM6-1_r1i1p1f2-CALIB</v>
       </c>
       <c r="C10" t="s">
         <v>1203</v>
@@ -17880,17 +17881,17 @@
         <v>1204</v>
       </c>
       <c r="E10" t="s">
-        <v>1220</v>
+        <v>1213</v>
       </c>
       <c r="F10">
-        <v>5.9849619111386696</v>
+        <v>8.1290947789614592</v>
       </c>
       <c r="G10">
-        <v>2.56750747873533</v>
+        <v>2.3996016020233899</v>
       </c>
       <c r="H10" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-NorCPM1_r1i1p1f1-CALIB</v>
+        <v>Model configuration tuned to CMIP6-CNRM-CM6-1_r1i1p1f2-CALIB</v>
       </c>
       <c r="J10" s="28" t="str">
         <f t="shared" si="2"/>
@@ -17906,7 +17907,7 @@
       <c r="A11" s="53"/>
       <c r="B11" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,2box,CMIP6-GISS-E2-1-G_r1i1p1f1-CALIB</v>
+        <v>ar5ir,2box,CMIP6-CNRM-ESM2-1_r1i1p1f2-CALIB</v>
       </c>
       <c r="C11" t="s">
         <v>1203</v>
@@ -17915,17 +17916,17 @@
         <v>1204</v>
       </c>
       <c r="E11" t="s">
-        <v>1217</v>
+        <v>1215</v>
       </c>
       <c r="F11">
-        <v>6.15826724672542</v>
+        <v>8.2189502610179694</v>
       </c>
       <c r="G11">
-        <v>1.84105608530307</v>
+        <v>2.23622944384873</v>
       </c>
       <c r="H11" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-GISS-E2-1-G_r1i1p1f1-CALIB</v>
+        <v>Model configuration tuned to CMIP6-CNRM-ESM2-1_r1i1p1f2-CALIB</v>
       </c>
       <c r="J11" s="28" t="str">
         <f t="shared" si="2"/>
@@ -17941,7 +17942,7 @@
       <c r="A12" s="53"/>
       <c r="B12" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,2box,CMIP6-BCC-ESM1_r1i1p1f1-CALIB</v>
+        <v>ar5ir,2box,CMIP6-CanESM5_r1i1p1f1-CALIB</v>
       </c>
       <c r="C12" t="s">
         <v>1203</v>
@@ -17950,17 +17951,17 @@
         <v>1204</v>
       </c>
       <c r="E12" t="s">
-        <v>1210</v>
+        <v>1214</v>
       </c>
       <c r="F12">
-        <v>6.1648418835021896</v>
+        <v>5.2355951793584001</v>
       </c>
       <c r="G12">
-        <v>2.77964097721043</v>
+        <v>2.8501811905871999</v>
       </c>
       <c r="H12" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-BCC-ESM1_r1i1p1f1-CALIB</v>
+        <v>Model configuration tuned to CMIP6-CanESM5_r1i1p1f1-CALIB</v>
       </c>
       <c r="J12" s="28" t="str">
         <f t="shared" si="2"/>
@@ -17976,26 +17977,26 @@
       <c r="A13" s="53"/>
       <c r="B13" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,3box,CMIP6-BCC-ESM1_r1i1p1f1-CALIB</v>
+        <v>ar5ir,2box,CMIP6-EC-Earth3-Veg_r1i1p1f1-CALIB</v>
       </c>
       <c r="C13" t="s">
         <v>1203</v>
       </c>
       <c r="D13" t="s">
-        <v>1208</v>
+        <v>1204</v>
       </c>
       <c r="E13" t="s">
-        <v>1210</v>
+        <v>1219</v>
       </c>
       <c r="F13">
-        <v>6.6063084373020704</v>
+        <v>15.908951471785899</v>
       </c>
       <c r="G13">
-        <v>2.22838284355496</v>
+        <v>2.63036743165426</v>
       </c>
       <c r="H13" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-BCC-ESM1_r1i1p1f1-CALIB</v>
+        <v>Model configuration tuned to CMIP6-EC-Earth3-Veg_r1i1p1f1-CALIB</v>
       </c>
       <c r="J13" s="28" t="str">
         <f t="shared" si="2"/>
@@ -18011,26 +18012,26 @@
       <c r="A14" s="38"/>
       <c r="B14" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,3box,CMIP6-MPI-ESM1-2-HR_r1i1p1f1-CALIB</v>
+        <v>ar5ir,2box,CMIP6-GISS-E2-1-G_r1i1p1f1-CALIB</v>
       </c>
       <c r="C14" t="s">
         <v>1203</v>
       </c>
       <c r="D14" t="s">
-        <v>1208</v>
+        <v>1204</v>
       </c>
       <c r="E14" t="s">
-        <v>1212</v>
+        <v>1217</v>
       </c>
       <c r="F14">
-        <v>6.7808043875969304</v>
+        <v>5.2388983939601896</v>
       </c>
       <c r="G14">
-        <v>1.5018336488069499</v>
+        <v>1.7329050551882601</v>
       </c>
       <c r="H14" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-MPI-ESM1-2-HR_r1i1p1f1-CALIB</v>
+        <v>Model configuration tuned to CMIP6-GISS-E2-1-G_r1i1p1f1-CALIB</v>
       </c>
       <c r="J14" s="28" t="str">
         <f t="shared" si="2"/>
@@ -18045,7 +18046,7 @@
     <row r="15" spans="1:91" ht="36.75" customHeight="1" thickBot="1">
       <c r="B15" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,2box,CMIP6-MPI-ESM1-2-HR_r1i1p1f1-CALIB</v>
+        <v>ar5ir,2box,CMIP6-GISS-E2-1-H_r1i1p1f1-CALIB</v>
       </c>
       <c r="C15" t="s">
         <v>1203</v>
@@ -18054,17 +18055,17 @@
         <v>1204</v>
       </c>
       <c r="E15" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="F15">
-        <v>6.7975907508722999</v>
+        <v>16.676179262476399</v>
       </c>
       <c r="G15">
-        <v>1.9159176016136701</v>
+        <v>1.9062682649690801</v>
       </c>
       <c r="H15" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-MPI-ESM1-2-HR_r1i1p1f1-CALIB</v>
+        <v>Model configuration tuned to CMIP6-GISS-E2-1-H_r1i1p1f1-CALIB</v>
       </c>
       <c r="J15" s="28" t="str">
         <f t="shared" si="2"/>
@@ -18078,7 +18079,7 @@
     <row r="16" spans="1:91" ht="36.75" customHeight="1" thickBot="1">
       <c r="B16" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,2box,CMIP6-GISS-E2-1-H_r1i1p1f1-CALIB</v>
+        <v>ar5ir,2box,CMIP6-GISS-E2-2-G_r1i1p1f1-CALIB</v>
       </c>
       <c r="C16" t="s">
         <v>1203</v>
@@ -18087,17 +18088,17 @@
         <v>1204</v>
       </c>
       <c r="E16" t="s">
-        <v>1211</v>
+        <v>1221</v>
       </c>
       <c r="F16">
-        <v>6.86884689256072</v>
+        <v>3.7033722822287398</v>
       </c>
       <c r="G16">
-        <v>2.3095936378866702</v>
+        <v>1.6556011325289799</v>
       </c>
       <c r="H16" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-GISS-E2-1-H_r1i1p1f1-CALIB</v>
+        <v>Model configuration tuned to CMIP6-GISS-E2-2-G_r1i1p1f1-CALIB</v>
       </c>
       <c r="J16" s="28" t="str">
         <f t="shared" si="2"/>
@@ -18111,26 +18112,26 @@
     <row r="17" spans="2:11" ht="36.75" customHeight="1" thickBot="1">
       <c r="B17" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,3box,CMIP6-GISS-E2-1-H_r1i1p1f1-CALIB</v>
+        <v>ar5ir,2box,CMIP6-IPSL-CM6A-LR_r1i1p1f1-CALIB</v>
       </c>
       <c r="C17" t="s">
         <v>1203</v>
       </c>
       <c r="D17" t="s">
-        <v>1208</v>
+        <v>1204</v>
       </c>
       <c r="E17" t="s">
-        <v>1211</v>
+        <v>1216</v>
       </c>
       <c r="F17">
-        <v>7.0265561916764101</v>
+        <v>13.569583760527401</v>
       </c>
       <c r="G17">
-        <v>1.69960479936043</v>
+        <v>2.5058283329328699</v>
       </c>
       <c r="H17" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-GISS-E2-1-H_r1i1p1f1-CALIB</v>
+        <v>Model configuration tuned to CMIP6-IPSL-CM6A-LR_r1i1p1f1-CALIB</v>
       </c>
       <c r="J17" s="28" t="str">
         <f t="shared" si="2"/>
@@ -18144,26 +18145,26 @@
     <row r="18" spans="2:11" ht="36.75" customHeight="1" thickBot="1">
       <c r="B18" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,3box,CMIP6-BCC-CSM2-MR_r1i1p1f1-CALIB</v>
+        <v>ar5ir,2box,CMIP6-MPI-ESM1-2-HR_r1i1p1f1-CALIB</v>
       </c>
       <c r="C18" t="s">
         <v>1203</v>
       </c>
       <c r="D18" t="s">
-        <v>1208</v>
+        <v>1204</v>
       </c>
       <c r="E18" t="s">
-        <v>1209</v>
+        <v>1212</v>
       </c>
       <c r="F18">
-        <v>7.1707996134210399</v>
+        <v>8.0183130287260909</v>
       </c>
       <c r="G18">
-        <v>1.8461789270732401</v>
+        <v>1.8464399568584999</v>
       </c>
       <c r="H18" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-BCC-CSM2-MR_r1i1p1f1-CALIB</v>
+        <v>Model configuration tuned to CMIP6-MPI-ESM1-2-HR_r1i1p1f1-CALIB</v>
       </c>
       <c r="J18" s="28" t="str">
         <f t="shared" si="2"/>
@@ -18177,7 +18178,7 @@
     <row r="19" spans="2:11" ht="36.75" customHeight="1" thickBot="1">
       <c r="B19" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,2box,CMIP6-BCC-CSM2-MR_r1i1p1f1-CALIB</v>
+        <v>ar5ir,2box,CMIP6-NorCPM1_r1i1p1f1-CALIB</v>
       </c>
       <c r="C19" t="s">
         <v>1203</v>
@@ -18186,17 +18187,17 @@
         <v>1204</v>
       </c>
       <c r="E19" t="s">
-        <v>1209</v>
+        <v>1220</v>
       </c>
       <c r="F19">
-        <v>7.4359428125203797</v>
+        <v>7.2376636605963904</v>
       </c>
       <c r="G19">
-        <v>1.8462748525833901</v>
+        <v>1.69888547776694</v>
       </c>
       <c r="H19" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-BCC-CSM2-MR_r1i1p1f1-CALIB</v>
+        <v>Model configuration tuned to CMIP6-NorCPM1_r1i1p1f1-CALIB</v>
       </c>
       <c r="J19" s="28" t="str">
         <f t="shared" si="2"/>
@@ -18210,7 +18211,7 @@
     <row r="20" spans="2:11" ht="36.75" customHeight="1" thickBot="1">
       <c r="B20" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,2box,CMIP6-CESM2-WACCM_r1i1p1f1-CALIB</v>
+        <v>ar5ir,2box,CMIP6-NorESM2-LM_r1i1p1f1-CALIB</v>
       </c>
       <c r="C20" t="s">
         <v>1203</v>
@@ -18219,17 +18220,17 @@
         <v>1204</v>
       </c>
       <c r="E20" t="s">
-        <v>1224</v>
+        <v>1222</v>
       </c>
       <c r="F20">
-        <v>7.4897386925168199</v>
+        <v>13.372198117051401</v>
       </c>
       <c r="G20">
-        <v>2.7807782105611798</v>
+        <v>1.56033724667033</v>
       </c>
       <c r="H20" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-CESM2-WACCM_r1i1p1f1-CALIB</v>
+        <v>Model configuration tuned to CMIP6-NorESM2-LM_r1i1p1f1-CALIB</v>
       </c>
       <c r="J20" s="28" t="str">
         <f t="shared" si="2"/>
@@ -18243,7 +18244,7 @@
     <row r="21" spans="2:11" ht="36.75" customHeight="1" thickBot="1">
       <c r="B21" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,2box,CMIP6-CNRM-ESM2-1_r1i1p1f2-CALIB</v>
+        <v>ar5ir,2box,CMIP6-UKESM1-0-LL_r1i1p1f2-CALIB</v>
       </c>
       <c r="C21" t="s">
         <v>1203</v>
@@ -18252,17 +18253,17 @@
         <v>1204</v>
       </c>
       <c r="E21" t="s">
-        <v>1215</v>
+        <v>1218</v>
       </c>
       <c r="F21">
-        <v>7.8002326489343403</v>
+        <v>16.9166502819293</v>
       </c>
       <c r="G21">
-        <v>2.6353449263897999</v>
+        <v>2.88242203911298</v>
       </c>
       <c r="H21" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-CNRM-ESM2-1_r1i1p1f2-CALIB</v>
+        <v>Model configuration tuned to CMIP6-UKESM1-0-LL_r1i1p1f2-CALIB</v>
       </c>
       <c r="J21" s="28" t="str">
         <f t="shared" si="2"/>
@@ -18276,7 +18277,7 @@
     <row r="22" spans="2:11" ht="36.75" customHeight="1" thickBot="1">
       <c r="B22" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,3box,CMIP6-CNRM-ESM2-1_r1i1p1f2-CALIB</v>
+        <v>ar5ir,3box,CMIP6-BCC-CSM2-MR_r1i1p1f1-CALIB</v>
       </c>
       <c r="C22" t="s">
         <v>1203</v>
@@ -18285,17 +18286,17 @@
         <v>1208</v>
       </c>
       <c r="E22" t="s">
-        <v>1215</v>
+        <v>1209</v>
       </c>
       <c r="F22">
-        <v>7.9858149852556002</v>
+        <v>7.7772635221303803</v>
       </c>
       <c r="G22">
-        <v>2.2904223860864299</v>
+        <v>1.91517643770951</v>
       </c>
       <c r="H22" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-CNRM-ESM2-1_r1i1p1f2-CALIB</v>
+        <v>Model configuration tuned to CMIP6-BCC-CSM2-MR_r1i1p1f1-CALIB</v>
       </c>
       <c r="J22" s="28" t="str">
         <f t="shared" si="2"/>
@@ -18309,7 +18310,7 @@
     <row r="23" spans="2:11" ht="36.75" customHeight="1" thickBot="1">
       <c r="B23" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,3box,CMIP6-CESM2-WACCM_r1i1p1f1-CALIB</v>
+        <v>ar5ir,3box,CMIP6-BCC-ESM1_r1i1p1f1-CALIB</v>
       </c>
       <c r="C23" t="s">
         <v>1203</v>
@@ -18318,17 +18319,17 @@
         <v>1208</v>
       </c>
       <c r="E23" t="s">
-        <v>1224</v>
+        <v>1210</v>
       </c>
       <c r="F23">
-        <v>8.23432269905312</v>
+        <v>8.0562218053625099</v>
       </c>
       <c r="G23">
-        <v>1.81377275062766</v>
+        <v>1.83716716580602</v>
       </c>
       <c r="H23" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-CESM2-WACCM_r1i1p1f1-CALIB</v>
+        <v>Model configuration tuned to CMIP6-BCC-ESM1_r1i1p1f1-CALIB</v>
       </c>
       <c r="J23" s="28" t="str">
         <f t="shared" si="2"/>
@@ -18342,7 +18343,7 @@
     <row r="24" spans="2:11" ht="36.75" customHeight="1" thickBot="1">
       <c r="B24" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,3box,CMIP6-CESM2_r1i1p1f1-CALIB</v>
+        <v>ar5ir,3box,CMIP6-CESM2-WACCM_r1i1p1f1-CALIB</v>
       </c>
       <c r="C24" t="s">
         <v>1203</v>
@@ -18351,17 +18352,17 @@
         <v>1208</v>
       </c>
       <c r="E24" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="F24">
-        <v>8.3803876364999894</v>
+        <v>13.4243640553892</v>
       </c>
       <c r="G24">
-        <v>2.22681989607229</v>
+        <v>2.2459127414780502</v>
       </c>
       <c r="H24" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-CESM2_r1i1p1f1-CALIB</v>
+        <v>Model configuration tuned to CMIP6-CESM2-WACCM_r1i1p1f1-CALIB</v>
       </c>
       <c r="J24" s="28" t="str">
         <f t="shared" si="2"/>
@@ -18375,22 +18376,22 @@
     <row r="25" spans="2:11" ht="36.75" customHeight="1" thickBot="1">
       <c r="B25" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,2box,CMIP6-CESM2_r1i1p1f1-CALIB</v>
+        <v>ar5ir,3box,CMIP6-CESM2_r1i1p1f1-CALIB</v>
       </c>
       <c r="C25" t="s">
         <v>1203</v>
       </c>
       <c r="D25" t="s">
-        <v>1204</v>
+        <v>1208</v>
       </c>
       <c r="E25" t="s">
         <v>1223</v>
       </c>
       <c r="F25">
-        <v>8.5042228866140697</v>
+        <v>8.3090052848392908</v>
       </c>
       <c r="G25">
-        <v>1.60118864510188</v>
+        <v>2.3575234866730899</v>
       </c>
       <c r="H25" s="28" t="str">
         <f t="shared" si="1"/>
@@ -18420,10 +18421,10 @@
         <v>1213</v>
       </c>
       <c r="F26">
-        <v>8.8187245100804397</v>
+        <v>9.1167840795780197</v>
       </c>
       <c r="G26">
-        <v>1.51316220722272</v>
+        <v>2.39539196793163</v>
       </c>
       <c r="H26" s="28" t="str">
         <f t="shared" si="1"/>
@@ -18441,26 +18442,26 @@
     <row r="27" spans="2:11" ht="36.75" customHeight="1" thickBot="1">
       <c r="B27" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,2box,CMIP6-CNRM-CM6-1_r1i1p1f2-CALIB</v>
+        <v>ar5ir,3box,CMIP6-CNRM-ESM2-1_r1i1p1f2-CALIB</v>
       </c>
       <c r="C27" t="s">
         <v>1203</v>
       </c>
       <c r="D27" t="s">
-        <v>1204</v>
+        <v>1208</v>
       </c>
       <c r="E27" t="s">
-        <v>1213</v>
+        <v>1215</v>
       </c>
       <c r="F27">
-        <v>9.8651644421965798</v>
+        <v>12.1781501868865</v>
       </c>
       <c r="G27">
-        <v>2.52472104840722</v>
+        <v>2.2366736891974099</v>
       </c>
       <c r="H27" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-CNRM-CM6-1_r1i1p1f2-CALIB</v>
+        <v>Model configuration tuned to CMIP6-CNRM-ESM2-1_r1i1p1f2-CALIB</v>
       </c>
       <c r="J27" s="28" t="str">
         <f t="shared" si="2"/>
@@ -18474,26 +18475,26 @@
     <row r="28" spans="2:11" ht="36.75" customHeight="1" thickBot="1">
       <c r="B28" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,2box,CMIP6-IPSL-CM6A-LR_r1i1p1f1-CALIB</v>
+        <v>ar5ir,3box,CMIP6-CanESM5_r1i1p1f1-CALIB</v>
       </c>
       <c r="C28" t="s">
         <v>1203</v>
       </c>
       <c r="D28" t="s">
-        <v>1204</v>
+        <v>1208</v>
       </c>
       <c r="E28" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
       <c r="F28">
-        <v>10.051406813280201</v>
+        <v>11.824380584858</v>
       </c>
       <c r="G28">
-        <v>1.9103133233887899</v>
+        <v>2.85731693157549</v>
       </c>
       <c r="H28" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-IPSL-CM6A-LR_r1i1p1f1-CALIB</v>
+        <v>Model configuration tuned to CMIP6-CanESM5_r1i1p1f1-CALIB</v>
       </c>
       <c r="J28" s="28" t="str">
         <f t="shared" si="2"/>
@@ -18519,10 +18520,10 @@
         <v>1219</v>
       </c>
       <c r="F29">
-        <v>10.324524704285899</v>
+        <v>8.3226533525584596</v>
       </c>
       <c r="G29">
-        <v>2.8582182087247001</v>
+        <v>2.5435661692617701</v>
       </c>
       <c r="H29" s="28" t="str">
         <f t="shared" si="1"/>
@@ -18540,26 +18541,26 @@
     <row r="30" spans="2:11" ht="36.75" customHeight="1" thickBot="1">
       <c r="B30" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,2box,CMIP6-EC-Earth3-Veg_r1i1p1f1-CALIB</v>
+        <v>ar5ir,3box,CMIP6-GISS-E2-1-G_r1i1p1f1-CALIB</v>
       </c>
       <c r="C30" t="s">
         <v>1203</v>
       </c>
       <c r="D30" t="s">
-        <v>1204</v>
+        <v>1208</v>
       </c>
       <c r="E30" t="s">
-        <v>1219</v>
+        <v>1217</v>
       </c>
       <c r="F30">
-        <v>10.541577456198601</v>
+        <v>18.9848511390502</v>
       </c>
       <c r="G30">
-        <v>1.9463318253605699</v>
+        <v>1.3179418966444101</v>
       </c>
       <c r="H30" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-EC-Earth3-Veg_r1i1p1f1-CALIB</v>
+        <v>Model configuration tuned to CMIP6-GISS-E2-1-G_r1i1p1f1-CALIB</v>
       </c>
       <c r="J30" s="28" t="str">
         <f t="shared" si="2"/>
@@ -18573,7 +18574,7 @@
     <row r="31" spans="2:11" ht="36.75" customHeight="1" thickBot="1">
       <c r="B31" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,3box,CMIP6-IPSL-CM6A-LR_r1i1p1f1-CALIB</v>
+        <v>ar5ir,3box,CMIP6-GISS-E2-1-H_r1i1p1f1-CALIB</v>
       </c>
       <c r="C31" t="s">
         <v>1203</v>
@@ -18582,17 +18583,17 @@
         <v>1208</v>
       </c>
       <c r="E31" t="s">
-        <v>1216</v>
+        <v>1211</v>
       </c>
       <c r="F31">
-        <v>11.081261663595701</v>
+        <v>8.0545461137078895</v>
       </c>
       <c r="G31">
-        <v>2.5503548725385801</v>
+        <v>1.90974455654996</v>
       </c>
       <c r="H31" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-IPSL-CM6A-LR_r1i1p1f1-CALIB</v>
+        <v>Model configuration tuned to CMIP6-GISS-E2-1-H_r1i1p1f1-CALIB</v>
       </c>
       <c r="J31" s="28" t="str">
         <f t="shared" si="2"/>
@@ -18606,7 +18607,7 @@
     <row r="32" spans="2:11" ht="36.75" customHeight="1" thickBot="1">
       <c r="B32" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,3box,CMIP6-UKESM1-0-LL_r1i1p1f2-CALIB</v>
+        <v>ar5ir,3box,CMIP6-GISS-E2-2-G_r1i1p1f1-CALIB</v>
       </c>
       <c r="C32" t="s">
         <v>1203</v>
@@ -18615,17 +18616,17 @@
         <v>1208</v>
       </c>
       <c r="E32" t="s">
-        <v>1218</v>
+        <v>1221</v>
       </c>
       <c r="F32">
-        <v>11.121920885669599</v>
+        <v>18.858431277947201</v>
       </c>
       <c r="G32">
-        <v>2.85597762214273</v>
+        <v>1.2561922732190101</v>
       </c>
       <c r="H32" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-UKESM1-0-LL_r1i1p1f2-CALIB</v>
+        <v>Model configuration tuned to CMIP6-GISS-E2-2-G_r1i1p1f1-CALIB</v>
       </c>
       <c r="J32" s="28" t="str">
         <f t="shared" si="2"/>
@@ -18639,26 +18640,26 @@
     <row r="33" spans="2:11" ht="36.75" customHeight="1" thickBot="1">
       <c r="B33" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,2box,CMIP6-CanESM5_r1i1p1f1-CALIB</v>
+        <v>ar5ir,3box,CMIP6-IPSL-CM6A-LR_r1i1p1f1-CALIB</v>
       </c>
       <c r="C33" t="s">
         <v>1203</v>
       </c>
       <c r="D33" t="s">
-        <v>1204</v>
+        <v>1208</v>
       </c>
       <c r="E33" t="s">
-        <v>1214</v>
+        <v>1216</v>
       </c>
       <c r="F33">
-        <v>11.3932405906894</v>
+        <v>5.70919768515021</v>
       </c>
       <c r="G33">
-        <v>2.3995591367559701</v>
+        <v>2.7157794824203698</v>
       </c>
       <c r="H33" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-CanESM5_r1i1p1f1-CALIB</v>
+        <v>Model configuration tuned to CMIP6-IPSL-CM6A-LR_r1i1p1f1-CALIB</v>
       </c>
       <c r="J33" s="28" t="str">
         <f t="shared" si="2"/>
@@ -18672,7 +18673,7 @@
     <row r="34" spans="2:11" ht="36.75" customHeight="1" thickBot="1">
       <c r="B34" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,3box,CMIP6-CanESM5_r1i1p1f1-CALIB</v>
+        <v>ar5ir,3box,CMIP6-MPI-ESM1-2-HR_r1i1p1f1-CALIB</v>
       </c>
       <c r="C34" t="s">
         <v>1203</v>
@@ -18681,17 +18682,17 @@
         <v>1208</v>
       </c>
       <c r="E34" t="s">
-        <v>1214</v>
+        <v>1212</v>
       </c>
       <c r="F34">
-        <v>11.487074387838099</v>
+        <v>6.0784829230164004</v>
       </c>
       <c r="G34">
-        <v>2.2471400050820498</v>
+        <v>1.84547214708943</v>
       </c>
       <c r="H34" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-CanESM5_r1i1p1f1-CALIB</v>
+        <v>Model configuration tuned to CMIP6-MPI-ESM1-2-HR_r1i1p1f1-CALIB</v>
       </c>
       <c r="J34" s="28" t="str">
         <f t="shared" si="2"/>
@@ -18702,29 +18703,29 @@
         <v>AR5 WG1 Ch.8 SM</v>
       </c>
     </row>
-    <row r="35" spans="2:11" ht="36.75" customHeight="1">
+    <row r="35" spans="2:11" ht="36.75" customHeight="1" thickBot="1">
       <c r="B35" s="54" t="str">
         <f t="shared" si="0"/>
-        <v>ar5ir,2box,CMIP6-UKESM1-0-LL_r1i1p1f2-CALIB</v>
+        <v>ar5ir,3box,CMIP6-NorCPM1_r1i1p1f1-CALIB</v>
       </c>
       <c r="C35" t="s">
         <v>1203</v>
       </c>
       <c r="D35" t="s">
-        <v>1204</v>
+        <v>1208</v>
       </c>
       <c r="E35" t="s">
-        <v>1218</v>
+        <v>1220</v>
       </c>
       <c r="F35">
-        <v>12.142995499498401</v>
+        <v>8.6011480648714205</v>
       </c>
       <c r="G35">
-        <v>2.3713783208676902</v>
+        <v>1.6323590388450999</v>
       </c>
       <c r="H35" s="28" t="str">
         <f t="shared" si="1"/>
-        <v>Model configuration tuned to CMIP6-UKESM1-0-LL_r1i1p1f2-CALIB</v>
+        <v>Model configuration tuned to CMIP6-NorCPM1_r1i1p1f1-CALIB</v>
       </c>
       <c r="J35" s="28" t="str">
         <f t="shared" si="2"/>
@@ -18735,8 +18736,72 @@
         <v>AR5 WG1 Ch.8 SM</v>
       </c>
     </row>
-    <row r="36" spans="2:11" ht="36.75" customHeight="1"/>
-    <row r="37" spans="2:11" ht="36.75" customHeight="1"/>
+    <row r="36" spans="2:11" ht="36.75" customHeight="1" thickBot="1">
+      <c r="B36" s="54" t="str">
+        <f t="shared" si="0"/>
+        <v>ar5ir,3box,CMIP6-NorESM2-LM_r1i1p1f1-CALIB</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1203</v>
+      </c>
+      <c r="D36" t="s">
+        <v>1208</v>
+      </c>
+      <c r="E36" t="s">
+        <v>1222</v>
+      </c>
+      <c r="F36">
+        <v>12.483125126345699</v>
+      </c>
+      <c r="G36">
+        <v>1.57133677777812</v>
+      </c>
+      <c r="H36" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v>Model configuration tuned to CMIP6-NorESM2-LM_r1i1p1f1-CALIB</v>
+      </c>
+      <c r="J36" s="28" t="str">
+        <f t="shared" si="2"/>
+        <v>Zebedee Nicholls (zebedee.nicholls@climate-energy-college.org)</v>
+      </c>
+      <c r="K36" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v>AR5 WG1 Ch.8 SM</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" ht="36.75" customHeight="1">
+      <c r="B37" s="54" t="str">
+        <f t="shared" si="0"/>
+        <v>ar5ir,3box,CMIP6-UKESM1-0-LL_r1i1p1f2-CALIB</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1203</v>
+      </c>
+      <c r="D37" t="s">
+        <v>1208</v>
+      </c>
+      <c r="E37" t="s">
+        <v>1218</v>
+      </c>
+      <c r="F37">
+        <v>7.2150705829123796</v>
+      </c>
+      <c r="G37">
+        <v>2.7835022898890198</v>
+      </c>
+      <c r="H37" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v>Model configuration tuned to CMIP6-UKESM1-0-LL_r1i1p1f2-CALIB</v>
+      </c>
+      <c r="J37" s="28" t="str">
+        <f t="shared" si="2"/>
+        <v>Zebedee Nicholls (zebedee.nicholls@climate-energy-college.org)</v>
+      </c>
+      <c r="K37" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v>AR5 WG1 Ch.8 SM</v>
+      </c>
+    </row>
     <row r="38" spans="2:11" ht="36.75" customHeight="1"/>
     <row r="39" spans="2:11" ht="36.75" customHeight="1"/>
     <row r="40" spans="2:11" ht="36.75" customHeight="1"/>

</xml_diff>

<commit_message>
Update IPSL 3 box tuning
</commit_message>
<xml_diff>
--- a/notebooks/rcmip-data-submission-template-ar5ir.xlsx
+++ b/notebooks/rcmip-data-submission-template-ar5ir.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11208"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA983CA-A05D-0A4F-A822-C8EE36661313}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAEB9A03-118C-9548-868C-274057B20595}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" tabRatio="682" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4225,20 +4225,20 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -4635,25 +4635,25 @@
       <c r="B1" s="15"/>
     </row>
     <row r="2" spans="1:13" ht="47.25" customHeight="1">
-      <c r="A2" s="79" t="s">
+      <c r="A2" s="78" t="s">
         <v>234</v>
       </c>
-      <c r="B2" s="79"/>
+      <c r="B2" s="78"/>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:13" ht="35.75" customHeight="1">
-      <c r="A3" s="78" t="s">
+      <c r="A3" s="76" t="s">
         <v>235</v>
       </c>
-      <c r="B3" s="78"/>
+      <c r="B3" s="76"/>
     </row>
     <row r="4" spans="1:13" ht="61" customHeight="1">
-      <c r="A4" s="80" t="s">
+      <c r="A4" s="77" t="s">
         <v>236</v>
       </c>
-      <c r="B4" s="80"/>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
+      <c r="B4" s="77"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:13" s="4" customFormat="1" ht="6" customHeight="1">
@@ -4672,20 +4672,20 @@
       <c r="M5" s="3"/>
     </row>
     <row r="6" spans="1:13" ht="25.5" customHeight="1">
-      <c r="A6" s="77" t="s">
+      <c r="A6" s="80" t="s">
         <v>76</v>
       </c>
-      <c r="B6" s="77"/>
+      <c r="B6" s="80"/>
     </row>
     <row r="7" spans="1:13" ht="6" customHeight="1">
       <c r="A7" s="17"/>
       <c r="B7" s="17"/>
     </row>
     <row r="8" spans="1:13" s="4" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A8" s="78" t="s">
+      <c r="A8" s="76" t="s">
         <v>848</v>
       </c>
-      <c r="B8" s="78"/>
+      <c r="B8" s="76"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -4699,8 +4699,8 @@
       <c r="M8" s="3"/>
     </row>
     <row r="9" spans="1:13" s="4" customFormat="1" ht="6" customHeight="1">
-      <c r="A9" s="78"/>
-      <c r="B9" s="78"/>
+      <c r="A9" s="76"/>
+      <c r="B9" s="76"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -4714,10 +4714,10 @@
       <c r="M9" s="3"/>
     </row>
     <row r="10" spans="1:13" s="4" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A10" s="78" t="s">
+      <c r="A10" s="76" t="s">
         <v>992</v>
       </c>
-      <c r="B10" s="78"/>
+      <c r="B10" s="76"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -4731,8 +4731,8 @@
       <c r="M10" s="3"/>
     </row>
     <row r="11" spans="1:13" s="4" customFormat="1" ht="6" customHeight="1">
-      <c r="A11" s="78"/>
-      <c r="B11" s="78"/>
+      <c r="A11" s="76"/>
+      <c r="B11" s="76"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -4746,10 +4746,10 @@
       <c r="M11" s="3"/>
     </row>
     <row r="12" spans="1:13" s="4" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A12" s="78" t="s">
+      <c r="A12" s="76" t="s">
         <v>237</v>
       </c>
-      <c r="B12" s="78"/>
+      <c r="B12" s="76"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -4763,8 +4763,8 @@
       <c r="M12" s="3"/>
     </row>
     <row r="13" spans="1:13" s="4" customFormat="1" ht="6" customHeight="1">
-      <c r="A13" s="78"/>
-      <c r="B13" s="78"/>
+      <c r="A13" s="76"/>
+      <c r="B13" s="76"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -4778,10 +4778,10 @@
       <c r="M13" s="3"/>
     </row>
     <row r="14" spans="1:13" s="4" customFormat="1" ht="90" customHeight="1">
-      <c r="A14" s="78" t="s">
+      <c r="A14" s="76" t="s">
         <v>628</v>
       </c>
-      <c r="B14" s="78"/>
+      <c r="B14" s="76"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -4810,10 +4810,10 @@
       <c r="M15" s="3"/>
     </row>
     <row r="16" spans="1:13">
-      <c r="A16" s="77" t="s">
+      <c r="A16" s="80" t="s">
         <v>820</v>
       </c>
-      <c r="B16" s="77"/>
+      <c r="B16" s="80"/>
     </row>
     <row r="17" spans="1:2" ht="26.25" customHeight="1">
       <c r="A17" s="69" t="s">
@@ -4836,10 +4836,10 @@
       <c r="B19" s="17"/>
     </row>
     <row r="20" spans="1:2" ht="27.75" customHeight="1">
-      <c r="A20" s="78" t="s">
+      <c r="A20" s="76" t="s">
         <v>106</v>
       </c>
-      <c r="B20" s="78"/>
+      <c r="B20" s="76"/>
     </row>
     <row r="21" spans="1:2" ht="27.75" customHeight="1">
       <c r="A21" s="72"/>
@@ -4852,10 +4852,10 @@
       <c r="B22" s="72"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="78" t="s">
+      <c r="A23" s="76" t="s">
         <v>1176</v>
       </c>
-      <c r="B23" s="78"/>
+      <c r="B23" s="76"/>
     </row>
     <row r="24" spans="1:2" ht="27.75" customHeight="1">
       <c r="A24" s="68"/>
@@ -4868,10 +4868,10 @@
       <c r="B25" s="68"/>
     </row>
     <row r="26" spans="1:2" ht="88" customHeight="1">
-      <c r="A26" s="78" t="s">
+      <c r="A26" s="76" t="s">
         <v>1032</v>
       </c>
-      <c r="B26" s="78"/>
+      <c r="B26" s="76"/>
     </row>
     <row r="27" spans="1:2" ht="27.75" customHeight="1">
       <c r="A27" s="68"/>
@@ -4950,22 +4950,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A14:B14"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A16:B16"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B17" r:id="rId1" xr:uid="{688D9660-F982-E440-B8DB-8E4CDAF396B8}"/>
@@ -17384,7 +17384,9 @@
   </sheetPr>
   <dimension ref="A1:CM65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.6640625" defaultRowHeight="13"/>
   <cols>
@@ -18652,10 +18654,10 @@
         <v>1216</v>
       </c>
       <c r="F33">
-        <v>5.70919768515021</v>
+        <v>4.98719465813305</v>
       </c>
       <c r="G33">
-        <v>2.7157794824203698</v>
+        <v>2.4632902876584</v>
       </c>
       <c r="H33" s="28" t="str">
         <f t="shared" si="1"/>

</xml_diff>